<commit_message>
Auto-committed on 2022/01/14 週五
Former-commit-id: 57e805e67de7c67ebf90a7cfbe47b68751e0e46c
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -4178,7 +4178,7 @@
         <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L3-帳務作業\LoanBorMain.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4196,7 +4196,7 @@
         <f>HYPERLINK("[\\192.168.10.16\St1Share(NAS)\SKL\DB\GenTables\L3-帳務作業\LoanBorTx.xlsx]DBD!A1", "連結")</f>
         <v>連結</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="1" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/20 週四
Former-commit-id: c92a101d4f4d1a3094436e8bcde376a0ef0b031a
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">客戶交互運用檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年05月03日 15:50:54</t>
+    <t xml:space="preserve">2022年01月20日 10:39:31</t>
   </si>
   <si>
     <t xml:space="preserve">CustFin</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">客戶資料主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月19日 09:39:05</t>
+    <t xml:space="preserve">2022年01月20日 10:39:54</t>
   </si>
   <si>
     <t xml:space="preserve">CustNotice</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">客戶聯絡電話檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月12日 17:31:36</t>
+    <t xml:space="preserve">2022年01月20日 10:18:49</t>
   </si>
   <si>
     <t xml:space="preserve">FinReportCashFlow</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">客戶財務報表.財報品質</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月06日 13:34:24</t>
+    <t xml:space="preserve">2022年01月20日 10:19:22</t>
   </si>
   <si>
     <t xml:space="preserve">FinReportRate</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">擔保品-建物修改原因檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年07月14日 16:59:12</t>
+    <t xml:space="preserve">2022年01月20日 10:22:23</t>
   </si>
   <si>
     <t xml:space="preserve">ClEva</t>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">擔保品不動產檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月07日 10:56:27</t>
+    <t xml:space="preserve">2022年01月20日 10:23:13</t>
   </si>
   <si>
     <t xml:space="preserve">ClImmRankDetail</t>
@@ -248,7 +248,7 @@
     <t xml:space="preserve">擔保品-土地所有權人檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年08月17日 14:06:21</t>
+    <t xml:space="preserve">2022年01月20日 10:24:19</t>
   </si>
   <si>
     <t xml:space="preserve">ClLandReason</t>
@@ -257,7 +257,7 @@
     <t xml:space="preserve">擔保品-土地修改原因檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年04月23日 16:00:32</t>
+    <t xml:space="preserve">2022年01月20日 10:24:44</t>
   </si>
   <si>
     <t xml:space="preserve">ClMain</t>
@@ -275,7 +275,7 @@
     <t xml:space="preserve">擔保品動產檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年08月17日 00:28:51</t>
+    <t xml:space="preserve">2022年01月20日 10:25:35</t>
   </si>
   <si>
     <t xml:space="preserve">ClNoMap</t>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">清償作業檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月22日 14:52:44</t>
+    <t xml:space="preserve">2022年01月20日 10:36:21</t>
   </si>
   <si>
     <t xml:space="preserve">FacMain</t>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">商品參數主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月01日 15:00:00</t>
+    <t xml:space="preserve">2022年01月20日 10:37:15</t>
   </si>
   <si>
     <t xml:space="preserve">FacProdAcctFee</t>
@@ -419,7 +419,7 @@
     <t xml:space="preserve">商品參數副檔階梯式利率</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年12月11日 18:36:39</t>
+    <t xml:space="preserve">2022年01月20日 10:37:42</t>
   </si>
   <si>
     <t xml:space="preserve">FacRelation</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">法拍費用檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月10日 15:07:39</t>
+    <t xml:space="preserve">2022年01月20日 10:38:18</t>
   </si>
   <si>
     <t xml:space="preserve">ForeclosureFinished</t>
@@ -500,7 +500,7 @@
     <t xml:space="preserve">借款戶關係人/關係企業主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月19日 12:43:12</t>
+    <t xml:space="preserve">2022年01月20日 10:38:57</t>
   </si>
   <si>
     <t xml:space="preserve">L3-帳務作業</t>
@@ -512,7 +512,7 @@
     <t xml:space="preserve">放款約定還本檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月01日 10:59:17</t>
+    <t xml:space="preserve">2022年01月20日 10:39:16</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorMain</t>
@@ -521,7 +521,7 @@
     <t xml:space="preserve">放款主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月14日 12:51:16</t>
+    <t xml:space="preserve">2022年01月20日 10:42:24</t>
   </si>
   <si>
     <t xml:space="preserve">LoanBorTx</t>
@@ -530,7 +530,7 @@
     <t xml:space="preserve">放款交易內容檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月14日 11:45:40</t>
+    <t xml:space="preserve">2022年01月20日 10:43:18</t>
   </si>
   <si>
     <t xml:space="preserve">LoanCheque</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">支票檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月01日 14:40:38</t>
+    <t xml:space="preserve">2022年01月20日 10:44:03</t>
   </si>
   <si>
     <t xml:space="preserve">LoanIntDetail</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">計息明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年09月29日 11:23:24</t>
+    <t xml:space="preserve">2022年01月20日 10:44:20</t>
   </si>
   <si>
     <t xml:space="preserve">LoanNotYet</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">未齊件管理檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月13日 17:05:09</t>
+    <t xml:space="preserve">2022年01月20日 10:44:37</t>
   </si>
   <si>
     <t xml:space="preserve">LoanOverdue</t>
@@ -566,7 +566,7 @@
     <t xml:space="preserve">催收呆帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年04月28日 18:24:38</t>
+    <t xml:space="preserve">2022年01月20日 10:44:53</t>
   </si>
   <si>
     <t xml:space="preserve">LoanRateChange</t>
@@ -575,7 +575,7 @@
     <t xml:space="preserve">放款利率變動檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月03日 12:15:38</t>
+    <t xml:space="preserve">2022年01月20日 10:45:09</t>
   </si>
   <si>
     <t xml:space="preserve">LoanSynd</t>
@@ -605,7 +605,7 @@
     <t xml:space="preserve">ACH授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月16日 15:19:52</t>
+    <t xml:space="preserve">2022年01月20日 10:48:13</t>
   </si>
   <si>
     <t xml:space="preserve">AchAuthLogHistory</t>
@@ -614,7 +614,7 @@
     <t xml:space="preserve">ACH授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月16日 11:23:29</t>
+    <t xml:space="preserve">2022年01月20日 10:49:14</t>
   </si>
   <si>
     <t xml:space="preserve">AchDeductMedia</t>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月05日 12:47:01</t>
+    <t xml:space="preserve">2022年01月20日 10:57:04</t>
   </si>
   <si>
     <t xml:space="preserve">BankAuthAct</t>
@@ -632,7 +632,7 @@
     <t xml:space="preserve">銀扣授權帳號檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月09日 10:17:13</t>
+    <t xml:space="preserve">2022年01月20日 10:55:17</t>
   </si>
   <si>
     <t xml:space="preserve">BankDeductDtl</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">銀行扣款明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月19日 11:23:26</t>
+    <t xml:space="preserve">2022年01月20日 10:58:09</t>
   </si>
   <si>
     <t xml:space="preserve">BankRemit</t>
@@ -650,7 +650,7 @@
     <t xml:space="preserve">撥款匯款檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月28日 11:52:15</t>
+    <t xml:space="preserve">2022年01月20日 10:59:19</t>
   </si>
   <si>
     <t xml:space="preserve">BankRmtf</t>
@@ -659,7 +659,7 @@
     <t xml:space="preserve">匯款轉帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年07月29日 16:48:08</t>
+    <t xml:space="preserve">2022年01月20日 10:59:49</t>
   </si>
   <si>
     <t xml:space="preserve">BatxCheque</t>
@@ -668,7 +668,7 @@
     <t xml:space="preserve">支票兌現檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月16日 19:06:16</t>
+    <t xml:space="preserve">2022年01月20日 11:00:17</t>
   </si>
   <si>
     <t xml:space="preserve">BatxDetail</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">整批入帳總數檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月02日 18:04:53</t>
+    <t xml:space="preserve">2022年01月20日 11:00:42</t>
   </si>
   <si>
     <t xml:space="preserve">BatxOthers</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">其他還款來源檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月06日 15:25:10</t>
+    <t xml:space="preserve">2022年01月20日 11:00:58</t>
   </si>
   <si>
     <t xml:space="preserve">BatxRateChange</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">整批利率調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月16日 16:25:48</t>
+    <t xml:space="preserve">2022年01月20日 11:01:44</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductDtl</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">員工扣薪明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月01日 17:20:13</t>
+    <t xml:space="preserve">2022年01月20日 11:02:26</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductMedia</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">員工扣薪媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月05日 17:28:39</t>
+    <t xml:space="preserve">2022年01月20日 11:03:12</t>
   </si>
   <si>
     <t xml:space="preserve">EmpDeductSchedule</t>
@@ -749,7 +749,7 @@
     <t xml:space="preserve">火險初保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月29日 11:01:15</t>
+    <t xml:space="preserve">2022年01月20日 11:03:31</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenew</t>
@@ -758,7 +758,7 @@
     <t xml:space="preserve">火險單續保檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月29日 11:01:35</t>
+    <t xml:space="preserve">2022年01月20日 11:03:54</t>
   </si>
   <si>
     <t xml:space="preserve">InsuRenewMediaTemp</t>
@@ -776,7 +776,7 @@
     <t xml:space="preserve">郵局授權記錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月27日 18:33:04</t>
+    <t xml:space="preserve">2022年01月20日 11:05:21</t>
   </si>
   <si>
     <t xml:space="preserve">PostAuthLogHistory</t>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">郵局授權記錄歷史檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月22日 10:47:38</t>
+    <t xml:space="preserve">2022年01月20日 11:06:26</t>
   </si>
   <si>
     <t xml:space="preserve">PostDeductMedia</t>
@@ -794,7 +794,7 @@
     <t xml:space="preserve">郵局扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月05日 12:47:06</t>
+    <t xml:space="preserve">2022年01月20日 11:07:17</t>
   </si>
   <si>
     <t xml:space="preserve">RepayActChangeLog</t>
@@ -803,7 +803,7 @@
     <t xml:space="preserve">還款帳號變更(含還款方式)紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月16日 12:13:35</t>
+    <t xml:space="preserve">2022年01月20日 11:07:45</t>
   </si>
   <si>
     <t xml:space="preserve">L5-管理性作業</t>
@@ -815,7 +815,7 @@
     <t xml:space="preserve">法催紀錄法務進度檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月22日 15:10:50</t>
+    <t xml:space="preserve">2022年01月20日 11:19:19</t>
   </si>
   <si>
     <t xml:space="preserve">CollLetter</t>
@@ -833,7 +833,7 @@
     <t xml:space="preserve">法催紀錄清單檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月11日 17:21:03</t>
+    <t xml:space="preserve">2022年01月20日 11:20:01</t>
   </si>
   <si>
     <t xml:space="preserve">CollListTmp</t>
@@ -860,7 +860,7 @@
     <t xml:space="preserve">法催紀錄提醒事項檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月28日 17:27:15</t>
+    <t xml:space="preserve">2022年01月20日 11:20:23</t>
   </si>
   <si>
     <t xml:space="preserve">CollTel</t>
@@ -932,7 +932,7 @@
     <t xml:space="preserve">檔案借閱檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月12日 13:50:38</t>
+    <t xml:space="preserve">2022年01月20日 11:21:28</t>
   </si>
   <si>
     <t xml:space="preserve">InnFundApl</t>
@@ -959,7 +959,7 @@
     <t xml:space="preserve">覆審案件明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月26日 15:06:38</t>
+    <t xml:space="preserve">2022年01月20日 11:22:18</t>
   </si>
   <si>
     <t xml:space="preserve">JcicAtomDetail</t>
@@ -1040,7 +1040,7 @@
     <t xml:space="preserve">債務協商案件主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月21日 19:04:28</t>
+    <t xml:space="preserve">2022年01月20日 11:24:01</t>
   </si>
   <si>
     <t xml:space="preserve">NegQueryCust</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">債協客戶請求資料</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年09月08日 14:18:41</t>
+    <t xml:space="preserve">2022年01月20日 11:26:29</t>
   </si>
   <si>
     <t xml:space="preserve">NegTrans</t>
@@ -1067,7 +1067,7 @@
     <t xml:space="preserve">房貸專員業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月18日 18:23:06</t>
+    <t xml:space="preserve">2022年01月20日 11:26:55</t>
   </si>
   <si>
     <t xml:space="preserve">PfBsDetailAdjust</t>
@@ -1094,7 +1094,7 @@
     <t xml:space="preserve">協辦人員等級檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年10月08日 16:04:37</t>
+    <t xml:space="preserve">2022年01月20日 11:27:22</t>
   </si>
   <si>
     <t xml:space="preserve">PfCoOfficerLog</t>
@@ -1121,7 +1121,7 @@
     <t xml:space="preserve">業績計算明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月02日 19:04:53</t>
+    <t xml:space="preserve">2022年01月20日 11:28:00</t>
   </si>
   <si>
     <t xml:space="preserve">PfInsCheck</t>
@@ -1130,7 +1130,7 @@
     <t xml:space="preserve">房貸獎勵保費檢核檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年05月03日 14:05:18</t>
+    <t xml:space="preserve">2022年01月20日 11:28:25</t>
   </si>
   <si>
     <t xml:space="preserve">PfIntranetAdjust</t>
@@ -1139,13 +1139,13 @@
     <t xml:space="preserve">內網報表業績調整檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年11月16日 14:21:26</t>
+    <t xml:space="preserve">2022年01月20日 11:28:43</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetail</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月16日 15:18:32</t>
+    <t xml:space="preserve">2022年01月20日 11:29:25</t>
   </si>
   <si>
     <t xml:space="preserve">PfItDetailAdjust</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/21 週五
Former-commit-id: 595db10e3144b8809ea6649506c0cfcde68c099d
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -677,7 +677,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 15:11:20</t>
+    <t xml:space="preserve">2022年01月21日 16:42:45</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -731,7 +731,7 @@
     <t xml:space="preserve">員工扣薪日程表</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年07月29日 18:28:44</t>
+    <t xml:space="preserve">2022年01月21日 16:55:08</t>
   </si>
   <si>
     <t xml:space="preserve">InsuComm</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/24 週一
Former-commit-id: 10a76d4fd3a109c1de379386590a3a409d61c933
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -794,7 +794,7 @@
     <t xml:space="preserve">郵局扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:07:17</t>
+    <t xml:space="preserve">2022年01月21日 17:31:20</t>
   </si>
   <si>
     <t xml:space="preserve">RepayActChangeLog</t>
@@ -914,7 +914,7 @@
     <t xml:space="preserve">介紹人業績明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月13日 10:19:23</t>
+    <t xml:space="preserve">2022年01月24日 11:14:15</t>
   </si>
   <si>
     <t xml:space="preserve">HlThreeLaqhcp</t>
@@ -1229,7 +1229,7 @@
     <t xml:space="preserve">會計業務關帳控制檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:31:18</t>
+    <t xml:space="preserve">2022年01月21日 17:25:28</t>
   </si>
   <si>
     <t xml:space="preserve">AcDetail</t>
@@ -1463,7 +1463,7 @@
     <t xml:space="preserve">編號編碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 15:07:19</t>
+    <t xml:space="preserve">2022年01月24日 10:38:10</t>
   </si>
   <si>
     <t xml:space="preserve">CdGuarantor</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/25 週二
Former-commit-id: b061e4509ee4a66d4077f824520bbb484a890afd
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -101,7 +101,7 @@
     <t xml:space="preserve">客戶聯絡電話檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月24日 11:36:19</t>
+    <t xml:space="preserve">2022年01月24日 18:06:58</t>
   </si>
   <si>
     <t xml:space="preserve">FinReportCashFlow</t>
@@ -1445,7 +1445,7 @@
     <t xml:space="preserve">共用代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:38:01</t>
+    <t xml:space="preserve">2022年01月25日 09:47:10</t>
   </si>
   <si>
     <t xml:space="preserve">CdEmp</t>
@@ -2900,7 +2900,7 @@
     <t xml:space="preserve">主管授權紀錄</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月24日 14:36:36</t>
+    <t xml:space="preserve">2022年01月24日 19:54:15</t>
   </si>
   <si>
     <t xml:space="preserve">TxBizDate</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/26 週三
Former-commit-id: 8e15f91e92cd29fe493e3aeaa3da1db18a87ac14
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -557,7 +557,7 @@
     <t xml:space="preserve">未齊件管理檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:44:37</t>
+    <t xml:space="preserve">2022年01月26日 09:37:17</t>
   </si>
   <si>
     <t xml:space="preserve">LoanOverdue</t>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 10:57:04</t>
+    <t xml:space="preserve">2022年01月26日 09:13:01</t>
   </si>
   <si>
     <t xml:space="preserve">BankAuthAct</t>
@@ -1274,7 +1274,7 @@
     <t xml:space="preserve">會計銷帳檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月24日 11:35:16</t>
+    <t xml:space="preserve">2022年01月26日 11:21:58</t>
   </si>
   <si>
     <t xml:space="preserve">CdAcBook</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/01/27 週四
Former-commit-id: b06ef90bad3d35fe040d9f145292189b3cc47037
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -623,7 +623,7 @@
     <t xml:space="preserve">ACH扣款媒體檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月26日 09:13:01</t>
+    <t xml:space="preserve">2022年01月27日 11:23:48</t>
   </si>
   <si>
     <t xml:space="preserve">BankAuthAct</t>
@@ -3023,7 +3023,7 @@
     <t xml:space="preserve">使用者檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2021年12月01日 17:20:37</t>
+    <t xml:space="preserve">2022年01月26日 17:24:05</t>
   </si>
   <si>
     <t xml:space="preserve">TxTellerAuth</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/02/09 週三
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -383,7 +383,7 @@
     <t xml:space="preserve">額度主檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月21日 15:00:35</t>
+    <t xml:space="preserve">2022年02月09日 09:24:25</t>
   </si>
   <si>
     <t xml:space="preserve">FacProd</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">整批入帳明細檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月21日 16:42:45</t>
+    <t xml:space="preserve">2022年02月08日 18:48:37</t>
   </si>
   <si>
     <t xml:space="preserve">BatxHead</t>
@@ -833,7 +833,7 @@
     <t xml:space="preserve">法催紀錄清單檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:20:01</t>
+    <t xml:space="preserve">2022年02月08日 19:26:06</t>
   </si>
   <si>
     <t xml:space="preserve">CollListTmp</t>
@@ -1445,7 +1445,7 @@
     <t xml:space="preserve">共用代碼檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月25日 09:47:10</t>
+    <t xml:space="preserve">2022年02月09日 13:42:09</t>
   </si>
   <si>
     <t xml:space="preserve">CdEmp</t>
@@ -2846,7 +2846,7 @@
     <t xml:space="preserve">ApLog敏感資料查詢紀錄檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2020年08月31日 11:32:48</t>
+    <t xml:space="preserve">2022年02月09日 13:10:19</t>
   </si>
   <si>
     <t xml:space="preserve">TxApLogList</t>

</xml_diff>

<commit_message>
Auto-committed on 2022/02/10 週四
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/GenTable總表.xlsx
@@ -1691,7 +1691,7 @@
     <t xml:space="preserve">違約損失率檔</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 11:52:30</t>
+    <t xml:space="preserve">2022年02月09日 17:51:58</t>
   </si>
   <si>
     <t xml:space="preserve">Ias39Loan34Data</t>
@@ -2771,7 +2771,7 @@
     <t xml:space="preserve">傳票媒體檔2022年格式</t>
   </si>
   <si>
-    <t xml:space="preserve">2022年01月20日 12:46:57</t>
+    <t xml:space="preserve">2022年02月09日 18:42:26</t>
   </si>
   <si>
     <t xml:space="preserve">UspErrorLog</t>

</xml_diff>